<commit_message>
Modified format of input data
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -7,8 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Assignments" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Counts" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Schedule" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -56,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -426,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:B80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,34 +450,28 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2024-08-16</t>
-        </is>
+      <c r="A2" s="2" t="n">
+        <v>45524</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Zoya</t>
+          <t>Sadaf</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2024-08-17</t>
-        </is>
+      <c r="A3" s="2" t="n">
+        <v>45525</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Zoya</t>
+          <t>Rachel</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2024-08-18</t>
-        </is>
+      <c r="A4" s="2" t="n">
+        <v>45526</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -483,22 +480,18 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2024-08-19</t>
-        </is>
+      <c r="A5" s="2" t="n">
+        <v>45527</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Zoya</t>
+          <t>Sadaf</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2024-08-20</t>
-        </is>
+      <c r="A6" s="2" t="n">
+        <v>45528</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -507,82 +500,68 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2024-08-21</t>
-        </is>
+      <c r="A7" s="2" t="n">
+        <v>45529</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Zoya</t>
+          <t>Rachel</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2024-08-22</t>
-        </is>
+      <c r="A8" s="2" t="n">
+        <v>45531</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Sadaf</t>
+          <t>Jamie</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2024-08-23</t>
-        </is>
+      <c r="A9" s="2" t="n">
+        <v>45532</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Sadaf</t>
+          <t>Jamie</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2024-08-24</t>
-        </is>
+      <c r="A10" s="2" t="n">
+        <v>45533</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Sadaf</t>
+          <t>Zoya</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2024-08-25</t>
-        </is>
+      <c r="A11" s="2" t="n">
+        <v>45534</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Jamie</t>
+          <t>Zoya</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2024-08-26</t>
-        </is>
+      <c r="A12" s="2" t="n">
+        <v>45535</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Sadaf</t>
+          <t>Jamie</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2024-08-27</t>
-        </is>
+      <c r="A13" s="2" t="n">
+        <v>45536</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -591,10 +570,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2024-08-28</t>
-        </is>
+      <c r="A14" s="2" t="n">
+        <v>45537</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -603,34 +580,28 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2024-08-29</t>
-        </is>
+      <c r="A15" s="2" t="n">
+        <v>45539</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Jamie</t>
+          <t>Zoya</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2024-08-30</t>
-        </is>
+      <c r="A16" s="2" t="n">
+        <v>45540</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Zoya</t>
+          <t>Jamie</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2024-08-31</t>
-        </is>
+      <c r="A17" s="2" t="n">
+        <v>45543</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -639,34 +610,28 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>2024-09-01</t>
-        </is>
+      <c r="A18" s="2" t="n">
+        <v>45544</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Zoya</t>
+          <t>Jamie</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>2024-09-02</t>
-        </is>
+      <c r="A19" s="2" t="n">
+        <v>45546</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Jamie</t>
+          <t>Sadaf</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>2024-09-03</t>
-        </is>
+      <c r="A20" s="2" t="n">
+        <v>45547</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -675,22 +640,18 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>2024-09-04</t>
-        </is>
+      <c r="A21" s="2" t="n">
+        <v>45548</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Jamie</t>
+          <t>Sadaf</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>2024-09-05</t>
-        </is>
+      <c r="A22" s="2" t="n">
+        <v>45549</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -699,46 +660,38 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>2024-09-06</t>
-        </is>
+      <c r="A23" s="2" t="n">
+        <v>45550</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Sadaf</t>
+          <t>Jamie</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>2024-09-07</t>
-        </is>
+      <c r="A24" s="2" t="n">
+        <v>45551</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Sadaf</t>
+          <t>Jamie</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>2024-09-08</t>
-        </is>
+      <c r="A25" s="2" t="n">
+        <v>45553</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Zoya</t>
+          <t>Sadaf</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>2024-09-09</t>
-        </is>
+      <c r="A26" s="2" t="n">
+        <v>45554</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -747,58 +700,48 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>2024-09-10</t>
-        </is>
+      <c r="A27" s="2" t="n">
+        <v>45555</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Zoya</t>
+          <t>Rachel</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>2024-09-11</t>
-        </is>
+      <c r="A28" s="2" t="n">
+        <v>45556</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Zoya</t>
+          <t>Jamie</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>2024-09-12</t>
-        </is>
+      <c r="A29" s="2" t="n">
+        <v>45557</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Jamie</t>
+          <t>Rachel</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>2024-09-13</t>
-        </is>
+      <c r="A30" s="2" t="n">
+        <v>45558</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Zoya</t>
+          <t>Jamie</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>2024-09-14</t>
-        </is>
+      <c r="A31" s="2" t="n">
+        <v>45560</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -807,130 +750,108 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>2024-09-15</t>
-        </is>
+      <c r="A32" s="2" t="n">
+        <v>45561</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Zoya</t>
+          <t>Jamie</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>2024-09-16</t>
-        </is>
+      <c r="A33" s="2" t="n">
+        <v>45564</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Jamie</t>
+          <t>Zoya</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>2024-09-17</t>
-        </is>
+      <c r="A34" s="2" t="n">
+        <v>45565</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Zoya</t>
+          <t>Jamie</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>2024-09-18</t>
-        </is>
+      <c r="A35" s="2" t="n">
+        <v>45567</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Jamie</t>
+          <t>Sadaf</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>2024-09-19</t>
-        </is>
+      <c r="A36" s="2" t="n">
+        <v>45568</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Jamie</t>
+          <t>Zoya</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>2024-09-20</t>
-        </is>
+      <c r="A37" s="2" t="n">
+        <v>45569</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Jamie</t>
+          <t>Sadaf</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
+      <c r="A38" s="2" t="n">
+        <v>45570</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Jamie</t>
+          <t>Rachel</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>2024-09-22</t>
-        </is>
+      <c r="A39" s="2" t="n">
+        <v>45571</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Jamie</t>
+          <t>Zoya</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>2024-09-23</t>
-        </is>
+      <c r="A40" s="2" t="n">
+        <v>45572</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Jamie</t>
+          <t>Rachel</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>2024-09-24</t>
-        </is>
+      <c r="A41" s="2" t="n">
+        <v>45574</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Zoya</t>
+          <t>Sadaf</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>2024-09-25</t>
-        </is>
+      <c r="A42" s="2" t="n">
+        <v>45575</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -939,10 +860,8 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>2024-09-26</t>
-        </is>
+      <c r="A43" s="2" t="n">
+        <v>45576</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -951,10 +870,8 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>2024-09-27</t>
-        </is>
+      <c r="A44" s="2" t="n">
+        <v>45577</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -963,22 +880,18 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>2024-09-28</t>
-        </is>
+      <c r="A45" s="2" t="n">
+        <v>45578</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Sadaf</t>
+          <t>Rachel</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>2024-09-29</t>
-        </is>
+      <c r="A46" s="2" t="n">
+        <v>45579</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -987,90 +900,343 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>2024-09-30</t>
-        </is>
+      <c r="A47" s="2" t="n">
+        <v>45581</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Jamie</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Weekdays Assigned</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Weekends Assigned</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Jamie</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>14</v>
-      </c>
-      <c r="C2" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Sadaf</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>5</v>
-      </c>
-      <c r="C3" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Zoya</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>13</v>
-      </c>
-      <c r="C4" t="n">
-        <v>6</v>
+          <t>Sadaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="n">
+        <v>45582</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Zoya</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="n">
+        <v>45583</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Jamie</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="n">
+        <v>45584</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Rachel</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="n">
+        <v>45585</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Zoya</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="n">
+        <v>45586</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Jamie</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="n">
+        <v>45588</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Sadaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="n">
+        <v>45589</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Zoya</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Sadaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="n">
+        <v>45593</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Rachel</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="n">
+        <v>45595</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Sadaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="n">
+        <v>45596</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Zoya</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="n">
+        <v>45520</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Rachel</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="n">
+        <v>45522</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Rachel</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="n">
+        <v>45530</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Sadaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="n">
+        <v>45538</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Rachel</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="n">
+        <v>45541</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Sadaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="n">
+        <v>45545</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Zoya</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="2" t="n">
+        <v>45552</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Zoya</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="n">
+        <v>45559</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Sadaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="n">
+        <v>45562</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Rachel</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="n">
+        <v>45563</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Rachel</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="n">
+        <v>45566</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Sadaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="n">
+        <v>45573</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Rachel</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="n">
+        <v>45580</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>unassigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="n">
+        <v>45587</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>unassigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="n">
+        <v>45592</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Rachel</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="n">
+        <v>45594</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>unassigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="n">
+        <v>45523</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>unassigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="n">
+        <v>45542</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>unassigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="n">
+        <v>45521</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>unassigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="n">
+        <v>45591</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>unassigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="n">
+        <v>45597</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>unassigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="n">
+        <v>45598</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>unassigned</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sorted by date added
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanviamrit/Desktop/Halligan/projs/ra_schedule/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11A966F-CEB0-1D42-89CF-93A8F6C9A8C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDF05DC-A2D7-7D47-A6E1-5F87A5D0BD32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8180" yWindow="500" windowWidth="25420" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -34,13 +34,13 @@
     <t>unassigned</t>
   </si>
   <si>
-    <t>Zoya</t>
-  </si>
-  <si>
     <t>Sadaf</t>
   </si>
   <si>
     <t>Jamie</t>
+  </si>
+  <si>
+    <t>Zoya</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -446,7 +446,7 @@
         <v>45524</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -454,7 +454,7 @@
         <v>45525</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -462,7 +462,7 @@
         <v>45526</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -470,7 +470,7 @@
         <v>45527</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -478,7 +478,7 @@
         <v>45528</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -486,7 +486,7 @@
         <v>45529</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -502,7 +502,7 @@
         <v>45531</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -510,7 +510,7 @@
         <v>45532</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -518,7 +518,7 @@
         <v>45533</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -526,7 +526,7 @@
         <v>45534</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -534,7 +534,7 @@
         <v>45535</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -542,7 +542,7 @@
         <v>45536</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -558,7 +558,7 @@
         <v>45538</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -566,7 +566,7 @@
         <v>45539</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -574,7 +574,7 @@
         <v>45540</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -582,7 +582,7 @@
         <v>45541</v>
       </c>
       <c r="B21" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -606,7 +606,7 @@
         <v>45544</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -622,7 +622,7 @@
         <v>45546</v>
       </c>
       <c r="B26" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -630,7 +630,7 @@
         <v>45547</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -646,7 +646,7 @@
         <v>45549</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -654,7 +654,7 @@
         <v>45550</v>
       </c>
       <c r="B30" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -662,7 +662,7 @@
         <v>45551</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -670,7 +670,7 @@
         <v>45552</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -678,7 +678,7 @@
         <v>45553</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -686,7 +686,7 @@
         <v>45554</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -702,7 +702,7 @@
         <v>45556</v>
       </c>
       <c r="B36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -718,7 +718,7 @@
         <v>45558</v>
       </c>
       <c r="B38" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -726,7 +726,7 @@
         <v>45559</v>
       </c>
       <c r="B39" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -734,7 +734,7 @@
         <v>45560</v>
       </c>
       <c r="B40" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -750,7 +750,7 @@
         <v>45562</v>
       </c>
       <c r="B42" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -758,7 +758,7 @@
         <v>45563</v>
       </c>
       <c r="B43" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -766,7 +766,7 @@
         <v>45564</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -782,7 +782,7 @@
         <v>45566</v>
       </c>
       <c r="B46" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -798,7 +798,7 @@
         <v>45568</v>
       </c>
       <c r="B48" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -806,7 +806,7 @@
         <v>45569</v>
       </c>
       <c r="B49" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -814,7 +814,7 @@
         <v>45570</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -822,7 +822,7 @@
         <v>45571</v>
       </c>
       <c r="B51" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -830,7 +830,7 @@
         <v>45572</v>
       </c>
       <c r="B52" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -838,7 +838,7 @@
         <v>45573</v>
       </c>
       <c r="B53" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -846,7 +846,7 @@
         <v>45574</v>
       </c>
       <c r="B54" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -854,7 +854,7 @@
         <v>45575</v>
       </c>
       <c r="B55" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -862,7 +862,7 @@
         <v>45576</v>
       </c>
       <c r="B56" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -870,7 +870,7 @@
         <v>45577</v>
       </c>
       <c r="B57" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -878,7 +878,7 @@
         <v>45578</v>
       </c>
       <c r="B58" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -886,7 +886,7 @@
         <v>45579</v>
       </c>
       <c r="B59" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -894,7 +894,7 @@
         <v>45580</v>
       </c>
       <c r="B60" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -902,7 +902,7 @@
         <v>45581</v>
       </c>
       <c r="B61" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -910,7 +910,7 @@
         <v>45582</v>
       </c>
       <c r="B62" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -926,7 +926,7 @@
         <v>45584</v>
       </c>
       <c r="B64" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -934,7 +934,7 @@
         <v>45585</v>
       </c>
       <c r="B65" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -950,7 +950,7 @@
         <v>45587</v>
       </c>
       <c r="B67" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
@@ -958,7 +958,7 @@
         <v>45588</v>
       </c>
       <c r="B68" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
@@ -966,7 +966,7 @@
         <v>45589</v>
       </c>
       <c r="B69" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
@@ -974,7 +974,7 @@
         <v>45590</v>
       </c>
       <c r="B70" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
@@ -982,7 +982,7 @@
         <v>45591</v>
       </c>
       <c r="B71" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
@@ -990,7 +990,7 @@
         <v>45592</v>
       </c>
       <c r="B72" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
@@ -1006,7 +1006,7 @@
         <v>45594</v>
       </c>
       <c r="B74" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
@@ -1030,7 +1030,7 @@
         <v>45597</v>
       </c>
       <c r="B77" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
@@ -1038,7 +1038,7 @@
         <v>45598</v>
       </c>
       <c r="B78" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>